<commit_message>
Added new section on beam motion error and changed associated text in summary section.
</commit_message>
<xml_diff>
--- a/OtherMaterials/TotalSystematicErrorTable.xlsx
+++ b/OtherMaterials/TotalSystematicErrorTable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/NickPC/Documents/Graduation/Dissertation/OtherMaterials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{469856EA-11DD-414D-AC7F-B7F1EA74B086}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8393D0D7-C02D-4340-BC6C-B0367A78E47B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="1860" windowWidth="28040" windowHeight="17440" xr2:uid="{13A7CC7D-E5DD-B54B-89F5-9477BBEDF731}"/>
+    <workbookView xWindow="39900" yWindow="19100" windowWidth="28040" windowHeight="17440" xr2:uid="{13A7CC7D-E5DD-B54B-89F5-9477BBEDF731}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>Total systematic error table</t>
   </si>
@@ -103,6 +103,15 @@
   </si>
   <si>
     <t>Total quadrature sum</t>
+  </si>
+  <si>
+    <t>Stored beam motion</t>
+  </si>
+  <si>
+    <t>Quadrature sum (no stored beam motion)</t>
+  </si>
+  <si>
+    <t>Total quadrature sum (no beam motion)</t>
   </si>
 </sst>
 </file>
@@ -463,15 +472,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17BA3B4E-0A14-7A4E-8738-91C0E27ED45A}">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.33203125" customWidth="1"/>
+    <col min="1" max="1" width="36.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -480,7 +489,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -799,45 +808,104 @@
         <v>28.3</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>115</v>
+      </c>
+      <c r="C27">
+        <v>180</v>
+      </c>
+      <c r="D27">
+        <v>180</v>
+      </c>
+      <c r="E27">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>24</v>
       </c>
-      <c r="B28">
+      <c r="B29">
+        <f>SQRT(SUMSQ(B23:B27))</f>
+        <v>138.11792063305907</v>
+      </c>
+      <c r="C29">
+        <f>SQRT(SUMSQ(C23:C27))</f>
+        <v>190.44025309792045</v>
+      </c>
+      <c r="D29">
+        <f>SQRT(SUMSQ(D23:D27))</f>
+        <v>190.90408586512757</v>
+      </c>
+      <c r="E29">
+        <f>SQRT(SUMSQ(E23:E27))</f>
+        <v>195.99624996412558</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30">
         <f>SQRT(SUMSQ(B23:B26))</f>
         <v>76.495490063140323</v>
       </c>
-      <c r="C28">
-        <f t="shared" ref="C28:E28" si="1">SQRT(SUMSQ(C23:C26))</f>
+      <c r="C30">
+        <f t="shared" ref="C30:E30" si="1">SQRT(SUMSQ(C23:C26))</f>
         <v>62.189146963115675</v>
       </c>
-      <c r="D28">
+      <c r="D30">
         <f t="shared" si="1"/>
         <v>63.595361466069207</v>
       </c>
-      <c r="E28">
+      <c r="E30">
         <f t="shared" si="1"/>
         <v>77.553400957017999</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>25</v>
       </c>
-      <c r="B32">
-        <f>SQRT(SUMSQ(B19, B28))</f>
+      <c r="B33">
+        <f>SQRT(SUMSQ(B19, B29))</f>
+        <v>144.07706271298011</v>
+      </c>
+      <c r="C33">
+        <f t="shared" ref="C33:E34" si="2">SQRT(SUMSQ(C19, C29))</f>
+        <v>199.50310774521785</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="2"/>
+        <v>194.46799222494175</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="2"/>
+        <v>204.20281584738248</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>28</v>
+      </c>
+      <c r="B34">
+        <f>SQRT(SUMSQ(B19, B30))</f>
         <v>86.794009009838931</v>
       </c>
-      <c r="C32">
-        <f t="shared" ref="C32:E32" si="2">SQRT(SUMSQ(C19, C28))</f>
+      <c r="C34">
+        <f t="shared" ref="C34:E34" si="3">SQRT(SUMSQ(C19, C30))</f>
         <v>86.031912683608283</v>
       </c>
-      <c r="D32">
-        <f t="shared" si="2"/>
+      <c r="D34">
+        <f t="shared" si="3"/>
         <v>73.605706300530798</v>
       </c>
-      <c r="E32">
-        <f t="shared" si="2"/>
+      <c r="E34">
+        <f t="shared" si="3"/>
         <v>96.430233848103882</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Working on conclusions chapter, added digit to R in fit results to go to 0.1 ppb level.
</commit_message>
<xml_diff>
--- a/OtherMaterials/TotalSystematicErrorTable.xlsx
+++ b/OtherMaterials/TotalSystematicErrorTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/NickPC/Documents/Graduation/Dissertation/OtherMaterials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8393D0D7-C02D-4340-BC6C-B0367A78E47B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6751DFA-969C-A046-8226-502D9C1E6DD6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39900" yWindow="19100" windowWidth="28040" windowHeight="17440" xr2:uid="{13A7CC7D-E5DD-B54B-89F5-9477BBEDF731}"/>
+    <workbookView xWindow="38400" yWindow="19100" windowWidth="24000" windowHeight="17440" xr2:uid="{13A7CC7D-E5DD-B54B-89F5-9477BBEDF731}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
   <si>
     <t>Total systematic error table</t>
   </si>
@@ -112,6 +112,12 @@
   </si>
   <si>
     <t>Total quadrature sum (no beam motion)</t>
+  </si>
+  <si>
+    <t>Statistical errors</t>
+  </si>
+  <si>
+    <t>Total errors</t>
   </si>
 </sst>
 </file>
@@ -155,9 +161,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,28 +479,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17BA3B4E-0A14-7A4E-8738-91C0E27ED45A}">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="36.6640625" customWidth="1"/>
+    <col min="9" max="9" width="16.1640625" customWidth="1"/>
+    <col min="12" max="12" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="I1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -509,8 +535,20 @@
       <c r="E5" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="I5" s="2">
+        <v>1358.1</v>
+      </c>
+      <c r="J5" s="2">
+        <v>1411.2</v>
+      </c>
+      <c r="K5" s="2">
+        <v>903.3</v>
+      </c>
+      <c r="L5" s="2">
+        <v>639.29999999999995</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -527,7 +565,7 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -544,7 +582,7 @@
         <v>14.3</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -560,8 +598,11 @@
       <c r="E8">
         <v>5.3</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="I8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -578,7 +619,7 @@
         <v>43.6</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -594,8 +635,20 @@
       <c r="E10">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="I10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -612,7 +665,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -628,8 +681,24 @@
       <c r="E12">
         <v>4.3</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="I12">
+        <f>SQRT(SUMSQ(I5,B33))</f>
+        <v>1365.7209854139312</v>
+      </c>
+      <c r="J12">
+        <f t="shared" ref="J12:L12" si="0">SQRT(SUMSQ(J5,C33))</f>
+        <v>1425.2322372160968</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="0"/>
+        <v>923.99604436382731</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="0"/>
+        <v>671.12091309986749</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -646,7 +715,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -663,7 +732,7 @@
         <v>28.9</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -680,7 +749,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -723,15 +792,15 @@
         <v>41.007804135310636</v>
       </c>
       <c r="C19">
-        <f t="shared" ref="C19:E19" si="0">SQRT(SUMSQ(C6:C17))</f>
+        <f t="shared" ref="C19:E19" si="1">SQRT(SUMSQ(C6:C17))</f>
         <v>59.447455790807403</v>
       </c>
       <c r="D19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>37.05981651330724</v>
       </c>
       <c r="E19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>57.308463598320273</v>
       </c>
     </row>
@@ -855,15 +924,15 @@
         <v>76.495490063140323</v>
       </c>
       <c r="C30">
-        <f t="shared" ref="C30:E30" si="1">SQRT(SUMSQ(C23:C26))</f>
+        <f t="shared" ref="C30:E30" si="2">SQRT(SUMSQ(C23:C26))</f>
         <v>62.189146963115675</v>
       </c>
       <c r="D30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>63.595361466069207</v>
       </c>
       <c r="E30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>77.553400957017999</v>
       </c>
     </row>
@@ -876,15 +945,15 @@
         <v>144.07706271298011</v>
       </c>
       <c r="C33">
-        <f t="shared" ref="C33:E34" si="2">SQRT(SUMSQ(C19, C29))</f>
+        <f t="shared" ref="C33:E33" si="3">SQRT(SUMSQ(C19, C29))</f>
         <v>199.50310774521785</v>
       </c>
       <c r="D33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>194.46799222494175</v>
       </c>
       <c r="E33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>204.20281584738248</v>
       </c>
     </row>
@@ -897,15 +966,15 @@
         <v>86.794009009838931</v>
       </c>
       <c r="C34">
-        <f t="shared" ref="C34:E34" si="3">SQRT(SUMSQ(C19, C30))</f>
+        <f t="shared" ref="C34:E34" si="4">SQRT(SUMSQ(C19, C30))</f>
         <v>86.031912683608283</v>
       </c>
       <c r="D34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>73.605706300530798</v>
       </c>
       <c r="E34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>96.430233848103882</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Removed other latex warnings besides fast rotation citation.
</commit_message>
<xml_diff>
--- a/OtherMaterials/TotalSystematicErrorTable.xlsx
+++ b/OtherMaterials/TotalSystematicErrorTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/NickPC/Documents/Graduation/Dissertation/OtherMaterials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6751DFA-969C-A046-8226-502D9C1E6DD6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3FC127F-A707-E149-BEF5-E896C9A7433B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38400" yWindow="19100" windowWidth="24000" windowHeight="17440" xr2:uid="{13A7CC7D-E5DD-B54B-89F5-9477BBEDF731}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
   <si>
     <t>Total systematic error table</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>Total errors</t>
+  </si>
+  <si>
+    <t>Dataset combined</t>
   </si>
 </sst>
 </file>
@@ -479,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17BA3B4E-0A14-7A4E-8738-91C0E27ED45A}">
-  <dimension ref="A1:L34"/>
+  <dimension ref="A1:N34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -490,17 +493,21 @@
     <col min="1" max="1" width="36.6640625" customWidth="1"/>
     <col min="9" max="9" width="16.1640625" customWidth="1"/>
     <col min="12" max="12" width="11.83203125" customWidth="1"/>
+    <col min="14" max="14" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="I1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="I3" s="1" t="s">
         <v>2</v>
       </c>
@@ -514,12 +521,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -547,8 +554,12 @@
       <c r="L5" s="2">
         <v>639.29999999999995</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N5" s="2">
+        <f>SQRT(1/(1/(I5^2) + 1/(J5^2) +  1/(K5^2) +  1/(L5^2)))</f>
+        <v>460.45178553028433</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -565,7 +576,7 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -582,7 +593,7 @@
         <v>14.3</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -602,7 +613,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -619,7 +630,7 @@
         <v>43.6</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -648,7 +659,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -665,7 +676,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -697,8 +708,12 @@
         <f t="shared" si="0"/>
         <v>671.12091309986749</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N12" s="2">
+        <f>SQRT(1/(1/(I12^2) + 1/(J12^2) +  1/(K12^2) +  1/(L12^2)))</f>
+        <v>475.65440034408613</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -715,7 +730,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -732,7 +747,7 @@
         <v>28.9</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -749,7 +764,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
Updates to wa systematics chapter, fixing spacing of tables, removing textbf comments, updating beam motion systematic error, etc. Made appropriate adjustments to final systematics table and conclusions table.
</commit_message>
<xml_diff>
--- a/OtherMaterials/TotalSystematicErrorTable.xlsx
+++ b/OtherMaterials/TotalSystematicErrorTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/NickPC/Documents/Graduation/Dissertation/OtherMaterials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3FC127F-A707-E149-BEF5-E896C9A7433B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11584538-B61B-8846-87DB-850827F44712}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38400" yWindow="19100" windowWidth="24000" windowHeight="17440" xr2:uid="{13A7CC7D-E5DD-B54B-89F5-9477BBEDF731}"/>
   </bookViews>
@@ -485,7 +485,7 @@
   <dimension ref="A1:N34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -698,11 +698,11 @@
       </c>
       <c r="J12">
         <f t="shared" ref="J12:L12" si="0">SQRT(SUMSQ(J5,C33))</f>
-        <v>1425.2322372160968</v>
+        <v>1418.4893126139514</v>
       </c>
       <c r="K12">
         <f t="shared" si="0"/>
-        <v>923.99604436382731</v>
+        <v>913.56099413230197</v>
       </c>
       <c r="L12">
         <f t="shared" si="0"/>
@@ -710,7 +710,7 @@
       </c>
       <c r="N12" s="2">
         <f>SQRT(1/(1/(I12^2) + 1/(J12^2) +  1/(K12^2) +  1/(L12^2)))</f>
-        <v>475.65440034408613</v>
+        <v>473.96303880538278</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
@@ -900,10 +900,10 @@
         <v>115</v>
       </c>
       <c r="C27">
-        <v>180</v>
+        <v>115</v>
       </c>
       <c r="D27">
-        <v>180</v>
+        <v>115</v>
       </c>
       <c r="E27">
         <v>180</v>
@@ -919,11 +919,11 @@
       </c>
       <c r="C29">
         <f>SQRT(SUMSQ(C23:C27))</f>
-        <v>190.44025309792045</v>
+        <v>130.7382499500433</v>
       </c>
       <c r="D29">
         <f>SQRT(SUMSQ(D23:D27))</f>
-        <v>190.90408586512757</v>
+        <v>131.41297500627553</v>
       </c>
       <c r="E29">
         <f>SQRT(SUMSQ(E23:E27))</f>
@@ -961,11 +961,11 @@
       </c>
       <c r="C33">
         <f t="shared" ref="C33:E33" si="3">SQRT(SUMSQ(C19, C29))</f>
-        <v>199.50310774521785</v>
+        <v>143.61925358391193</v>
       </c>
       <c r="D33">
         <f t="shared" si="3"/>
-        <v>194.46799222494175</v>
+        <v>136.53863921981937</v>
       </c>
       <c r="E33">
         <f t="shared" si="3"/>

</xml_diff>

<commit_message>
Replaced 9d CBO C envelope number and error, removed k_loss paragraph for HighKick and Endgame datasets where I estimated the error with 2x IFG, fixed up errors in the E-field/pitch and updated tables and summary totals, moved differential decay section lower, etc.
</commit_message>
<xml_diff>
--- a/OtherMaterials/TotalSystematicErrorTable.xlsx
+++ b/OtherMaterials/TotalSystematicErrorTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/NickPC/Documents/Graduation/Dissertation/OtherMaterials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11584538-B61B-8846-87DB-850827F44712}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF9A6D4D-0B3C-F441-99A5-5EBBC87AFE00}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38400" yWindow="19100" windowWidth="24000" windowHeight="17440" xr2:uid="{13A7CC7D-E5DD-B54B-89F5-9477BBEDF731}"/>
   </bookViews>
@@ -485,7 +485,7 @@
   <dimension ref="A1:N34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -687,7 +687,7 @@
         <v>18</v>
       </c>
       <c r="D12">
-        <v>28.7</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="E12">
         <v>4.3</v>
@@ -698,19 +698,19 @@
       </c>
       <c r="J12">
         <f t="shared" ref="J12:L12" si="0">SQRT(SUMSQ(J5,C33))</f>
-        <v>1418.4893126139514</v>
+        <v>1417.9587899512453</v>
       </c>
       <c r="K12">
         <f t="shared" si="0"/>
-        <v>913.56099413230197</v>
+        <v>913.15742892449816</v>
       </c>
       <c r="L12">
         <f t="shared" si="0"/>
-        <v>671.12091309986749</v>
+        <v>670.49838180267068</v>
       </c>
       <c r="N12" s="2">
         <f>SQRT(1/(1/(I12^2) + 1/(J12^2) +  1/(K12^2) +  1/(L12^2)))</f>
-        <v>473.96303880538278</v>
+        <v>473.66753895508873</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
@@ -738,13 +738,13 @@
         <v>1.2</v>
       </c>
       <c r="C14">
-        <v>39.1</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="D14">
         <v>3.1</v>
       </c>
       <c r="E14">
-        <v>28.9</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
@@ -808,15 +808,15 @@
       </c>
       <c r="C19">
         <f t="shared" ref="C19:E19" si="1">SQRT(SUMSQ(C6:C17))</f>
-        <v>59.447455790807403</v>
+        <v>45.046642494197059</v>
       </c>
       <c r="D19">
         <f t="shared" si="1"/>
-        <v>37.05981651330724</v>
+        <v>25.223600060261024</v>
       </c>
       <c r="E19">
         <f t="shared" si="1"/>
-        <v>57.308463598320273</v>
+        <v>49.487978338178259</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -961,15 +961,15 @@
       </c>
       <c r="C33">
         <f t="shared" ref="C33:E33" si="3">SQRT(SUMSQ(C19, C29))</f>
-        <v>143.61925358391193</v>
+        <v>138.28119901129003</v>
       </c>
       <c r="D33">
         <f t="shared" si="3"/>
-        <v>136.53863921981937</v>
+        <v>133.81180814860846</v>
       </c>
       <c r="E33">
         <f t="shared" si="3"/>
-        <v>204.20281584738248</v>
+        <v>202.14744618718288</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
@@ -982,15 +982,15 @@
       </c>
       <c r="C34">
         <f t="shared" ref="C34:E34" si="4">SQRT(SUMSQ(C19, C30))</f>
-        <v>86.031912683608283</v>
+        <v>76.789908191115842</v>
       </c>
       <c r="D34">
         <f t="shared" si="4"/>
-        <v>73.605706300530798</v>
+        <v>68.414910655499654</v>
       </c>
       <c r="E34">
         <f t="shared" si="4"/>
-        <v>96.430233848103882</v>
+        <v>91.997771712145294</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Forgot to commit changes to excel error table.
</commit_message>
<xml_diff>
--- a/OtherMaterials/TotalSystematicErrorTable.xlsx
+++ b/OtherMaterials/TotalSystematicErrorTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/NickPC/Documents/Graduation/Dissertation/OtherMaterials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF9A6D4D-0B3C-F441-99A5-5EBBC87AFE00}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDEFD20A-47CF-0445-8E20-03095FEA2775}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38400" yWindow="19100" windowWidth="24000" windowHeight="17440" xr2:uid="{13A7CC7D-E5DD-B54B-89F5-9477BBEDF731}"/>
   </bookViews>
@@ -485,7 +485,7 @@
   <dimension ref="A1:N34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -694,23 +694,23 @@
       </c>
       <c r="I12">
         <f>SQRT(SUMSQ(I5,B33))</f>
-        <v>1365.7209854139312</v>
+        <v>1365.7119645078899</v>
       </c>
       <c r="J12">
         <f t="shared" ref="J12:L12" si="0">SQRT(SUMSQ(J5,C33))</f>
-        <v>1417.9587899512453</v>
+        <v>1417.9501013787474</v>
       </c>
       <c r="K12">
         <f t="shared" si="0"/>
-        <v>913.15742892449816</v>
+        <v>913.14393717529538</v>
       </c>
       <c r="L12">
         <f t="shared" si="0"/>
-        <v>670.49838180267068</v>
+        <v>670.48000715905016</v>
       </c>
       <c r="N12" s="2">
         <f>SQRT(1/(1/(I12^2) + 1/(J12^2) +  1/(K12^2) +  1/(L12^2)))</f>
-        <v>473.66753895508873</v>
+        <v>473.65847758830745</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
@@ -863,16 +863,16 @@
         <v>22</v>
       </c>
       <c r="B25">
-        <v>15.8</v>
+        <v>15</v>
       </c>
       <c r="C25">
-        <v>15.8</v>
+        <v>15</v>
       </c>
       <c r="D25">
-        <v>15.8</v>
+        <v>15</v>
       </c>
       <c r="E25">
-        <v>15.8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -915,19 +915,19 @@
       </c>
       <c r="B29">
         <f>SQRT(SUMSQ(B23:B27))</f>
-        <v>138.11792063305907</v>
+        <v>138.02869266931421</v>
       </c>
       <c r="C29">
         <f>SQRT(SUMSQ(C23:C27))</f>
-        <v>130.7382499500433</v>
+        <v>130.64398187440551</v>
       </c>
       <c r="D29">
         <f>SQRT(SUMSQ(D23:D27))</f>
-        <v>131.41297500627553</v>
+        <v>131.3191912859655</v>
       </c>
       <c r="E29">
         <f>SQRT(SUMSQ(E23:E27))</f>
-        <v>195.99624996412558</v>
+        <v>195.93338153566378</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -936,19 +936,19 @@
       </c>
       <c r="B30">
         <f>SQRT(SUMSQ(B23:B26))</f>
-        <v>76.495490063140323</v>
+        <v>76.334264914257218</v>
       </c>
       <c r="C30">
         <f t="shared" ref="C30:E30" si="2">SQRT(SUMSQ(C23:C26))</f>
-        <v>62.189146963115675</v>
+        <v>61.990725112713434</v>
       </c>
       <c r="D30">
         <f t="shared" si="2"/>
-        <v>63.595361466069207</v>
+        <v>63.401340679831058</v>
       </c>
       <c r="E30">
         <f t="shared" si="2"/>
-        <v>77.553400957017999</v>
+        <v>77.394379640901576</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
@@ -957,19 +957,19 @@
       </c>
       <c r="B33">
         <f>SQRT(SUMSQ(B19, B29))</f>
-        <v>144.07706271298011</v>
+        <v>143.99152752853203</v>
       </c>
       <c r="C33">
         <f t="shared" ref="C33:E33" si="3">SQRT(SUMSQ(C19, C29))</f>
-        <v>138.28119901129003</v>
+        <v>138.19207647329131</v>
       </c>
       <c r="D33">
         <f t="shared" si="3"/>
-        <v>133.81180814860846</v>
+        <v>133.71970684981326</v>
       </c>
       <c r="E33">
         <f t="shared" si="3"/>
-        <v>202.14744618718288</v>
+        <v>202.08649138425852</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
@@ -978,19 +978,19 @@
       </c>
       <c r="B34">
         <f>SQRT(SUMSQ(B19, B30))</f>
-        <v>86.794009009838931</v>
+        <v>86.651947468017141</v>
       </c>
       <c r="C34">
         <f t="shared" ref="C34:E34" si="4">SQRT(SUMSQ(C19, C30))</f>
-        <v>76.789908191115842</v>
+        <v>76.62930248932193</v>
       </c>
       <c r="D34">
         <f t="shared" si="4"/>
-        <v>68.414910655499654</v>
+        <v>68.234595331107514</v>
       </c>
       <c r="E34">
         <f t="shared" si="4"/>
-        <v>91.997771712145294</v>
+        <v>91.863757815582531</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Wrote about IFG lifetime error and included numbers in tables.
</commit_message>
<xml_diff>
--- a/OtherMaterials/TotalSystematicErrorTable.xlsx
+++ b/OtherMaterials/TotalSystematicErrorTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/NickPC/Documents/Graduation/Dissertation/OtherMaterials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDEFD20A-47CF-0445-8E20-03095FEA2775}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E252738-BCA6-834F-804D-A84D11F7DC1F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38400" yWindow="19100" windowWidth="24000" windowHeight="17440" xr2:uid="{13A7CC7D-E5DD-B54B-89F5-9477BBEDF731}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
   <si>
     <t>Total systematic error table</t>
   </si>
@@ -121,6 +121,9 @@
   </si>
   <si>
     <t>Dataset combined</t>
+  </si>
+  <si>
+    <t>In-fill gain lifetime</t>
   </si>
 </sst>
 </file>
@@ -482,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17BA3B4E-0A14-7A4E-8738-91C0E27ED45A}">
-  <dimension ref="A1:N34"/>
+  <dimension ref="A1:N35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -632,365 +635,382 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="B10">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C10">
-        <v>11</v>
+        <v>11.2</v>
       </c>
       <c r="D10">
-        <v>11</v>
+        <v>11.6</v>
       </c>
       <c r="E10">
-        <v>11</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>5</v>
+        <v>16.5</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11">
-        <v>7.5</v>
+        <v>11</v>
       </c>
       <c r="C11">
-        <v>0.4</v>
+        <v>11</v>
       </c>
       <c r="D11">
+        <v>11</v>
+      </c>
+      <c r="E11">
+        <v>11</v>
+      </c>
+      <c r="I11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E11">
-        <v>8</v>
+      <c r="J11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12">
-        <v>17.600000000000001</v>
+        <v>7.5</v>
       </c>
       <c r="C12">
-        <v>18</v>
+        <v>0.4</v>
       </c>
       <c r="D12">
-        <v>9.3000000000000007</v>
+        <v>2</v>
       </c>
       <c r="E12">
-        <v>4.3</v>
-      </c>
-      <c r="I12">
-        <f>SQRT(SUMSQ(I5,B33))</f>
-        <v>1365.7119645078899</v>
-      </c>
-      <c r="J12">
-        <f t="shared" ref="J12:L12" si="0">SQRT(SUMSQ(J5,C33))</f>
-        <v>1417.9501013787474</v>
-      </c>
-      <c r="K12">
-        <f t="shared" si="0"/>
-        <v>913.14393717529538</v>
-      </c>
-      <c r="L12">
-        <f t="shared" si="0"/>
-        <v>670.48000715905016</v>
-      </c>
-      <c r="N12" s="2">
-        <f>SQRT(1/(1/(I12^2) + 1/(J12^2) +  1/(K12^2) +  1/(L12^2)))</f>
-        <v>473.65847758830745</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13">
-        <v>0.5</v>
+        <v>17.600000000000001</v>
       </c>
       <c r="C13">
-        <v>0.5</v>
+        <v>18</v>
       </c>
       <c r="D13">
-        <v>0.5</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="E13">
-        <v>0.5</v>
+        <v>4.3</v>
+      </c>
+      <c r="I13">
+        <f>SQRT(SUMSQ(I5,B34))</f>
+        <v>1365.7211172124416</v>
+      </c>
+      <c r="J13">
+        <f t="shared" ref="J13:L13" si="0">SQRT(SUMSQ(J5,C34))</f>
+        <v>1417.9943335570845</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="0"/>
+        <v>913.21761371537286</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="0"/>
+        <v>670.68300261748095</v>
+      </c>
+      <c r="N13" s="2">
+        <f>SQRT(1/(1/(I13^2) + 1/(J13^2) +  1/(K13^2) +  1/(L13^2)))</f>
+        <v>473.74234828724633</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14">
-        <v>1.2</v>
+        <v>0.5</v>
       </c>
       <c r="C14">
-        <v>4.9000000000000004</v>
+        <v>0.5</v>
       </c>
       <c r="D14">
-        <v>3.1</v>
+        <v>0.5</v>
       </c>
       <c r="E14">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15">
-        <v>2.4</v>
+        <v>1.2</v>
       </c>
       <c r="C15">
-        <v>2.4</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="D15">
-        <v>2.4</v>
+        <v>3.1</v>
       </c>
       <c r="E15">
-        <v>2.4</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16">
-        <v>0.1</v>
+        <v>2.4</v>
       </c>
       <c r="C16">
-        <v>0.1</v>
+        <v>2.4</v>
       </c>
       <c r="D16">
-        <v>0.1</v>
+        <v>2.4</v>
       </c>
       <c r="E16">
-        <v>0.1</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17">
+        <v>0.1</v>
+      </c>
+      <c r="C17">
+        <v>0.1</v>
+      </c>
+      <c r="D17">
+        <v>0.1</v>
+      </c>
+      <c r="E17">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>19</v>
       </c>
-      <c r="B17">
+      <c r="B18">
         <v>2.5</v>
       </c>
-      <c r="C17">
+      <c r="C18">
         <v>0.6</v>
       </c>
-      <c r="D17">
+      <c r="D18">
         <v>2.2999999999999998</v>
       </c>
-      <c r="E17">
+      <c r="E18">
         <v>4.2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>24</v>
       </c>
-      <c r="B19">
-        <f>SQRT(SUMSQ(B6:B17))</f>
-        <v>41.007804135310636</v>
-      </c>
-      <c r="C19">
-        <f t="shared" ref="C19:E19" si="1">SQRT(SUMSQ(C6:C17))</f>
-        <v>45.046642494197059</v>
-      </c>
-      <c r="D19">
+      <c r="B20">
+        <f>SQRT(SUMSQ(B6:B18))</f>
+        <v>41.31149960967285</v>
+      </c>
+      <c r="C20">
+        <f t="shared" ref="C20:E20" si="1">SQRT(SUMSQ(C6:C18))</f>
+        <v>46.418099918027671</v>
+      </c>
+      <c r="D20">
         <f t="shared" si="1"/>
-        <v>25.223600060261024</v>
-      </c>
-      <c r="E19">
+        <v>27.76310501366877</v>
+      </c>
+      <c r="E20">
         <f t="shared" si="1"/>
-        <v>49.487978338178259</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
+        <v>52.16617678151237</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>20</v>
-      </c>
-      <c r="B23">
-        <v>53.6</v>
-      </c>
-      <c r="C23">
-        <v>17.899999999999999</v>
-      </c>
-      <c r="D23">
-        <v>22.3</v>
-      </c>
-      <c r="E23">
-        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B24">
-        <v>40</v>
+        <v>53.6</v>
       </c>
       <c r="C24">
-        <v>40</v>
+        <v>17.899999999999999</v>
       </c>
       <c r="D24">
-        <v>40</v>
+        <v>22.3</v>
       </c>
       <c r="E24">
-        <v>40</v>
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B25">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="C25">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="D25">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="E25">
-        <v>15</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B26">
-        <v>33.6</v>
+        <v>15</v>
       </c>
       <c r="C26">
-        <v>41.2</v>
+        <v>15</v>
       </c>
       <c r="D26">
-        <v>41.2</v>
+        <v>15</v>
       </c>
       <c r="E26">
-        <v>28.3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27">
+        <v>33.6</v>
+      </c>
+      <c r="C27">
+        <v>41.2</v>
+      </c>
+      <c r="D27">
+        <v>41.2</v>
+      </c>
+      <c r="E27">
+        <v>28.3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>26</v>
       </c>
-      <c r="B27">
+      <c r="B28">
         <v>115</v>
       </c>
-      <c r="C27">
+      <c r="C28">
         <v>115</v>
       </c>
-      <c r="D27">
+      <c r="D28">
         <v>115</v>
       </c>
-      <c r="E27">
+      <c r="E28">
         <v>180</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>24</v>
-      </c>
-      <c r="B29">
-        <f>SQRT(SUMSQ(B23:B27))</f>
-        <v>138.02869266931421</v>
-      </c>
-      <c r="C29">
-        <f>SQRT(SUMSQ(C23:C27))</f>
-        <v>130.64398187440551</v>
-      </c>
-      <c r="D29">
-        <f>SQRT(SUMSQ(D23:D27))</f>
-        <v>131.3191912859655</v>
-      </c>
-      <c r="E29">
-        <f>SQRT(SUMSQ(E23:E27))</f>
-        <v>195.93338153566378</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
+        <v>24</v>
+      </c>
+      <c r="B30">
+        <f>SQRT(SUMSQ(B24:B28))</f>
+        <v>138.02869266931421</v>
+      </c>
+      <c r="C30">
+        <f>SQRT(SUMSQ(C24:C28))</f>
+        <v>130.64398187440551</v>
+      </c>
+      <c r="D30">
+        <f>SQRT(SUMSQ(D24:D28))</f>
+        <v>131.3191912859655</v>
+      </c>
+      <c r="E30">
+        <f>SQRT(SUMSQ(E24:E28))</f>
+        <v>195.93338153566378</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>27</v>
       </c>
-      <c r="B30">
-        <f>SQRT(SUMSQ(B23:B26))</f>
+      <c r="B31">
+        <f>SQRT(SUMSQ(B24:B27))</f>
         <v>76.334264914257218</v>
       </c>
-      <c r="C30">
-        <f t="shared" ref="C30:E30" si="2">SQRT(SUMSQ(C23:C26))</f>
+      <c r="C31">
+        <f t="shared" ref="C31:E31" si="2">SQRT(SUMSQ(C24:C27))</f>
         <v>61.990725112713434</v>
       </c>
-      <c r="D30">
+      <c r="D31">
         <f t="shared" si="2"/>
         <v>63.401340679831058</v>
       </c>
-      <c r="E30">
+      <c r="E31">
         <f t="shared" si="2"/>
         <v>77.394379640901576</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>25</v>
-      </c>
-      <c r="B33">
-        <f>SQRT(SUMSQ(B19, B29))</f>
-        <v>143.99152752853203</v>
-      </c>
-      <c r="C33">
-        <f t="shared" ref="C33:E33" si="3">SQRT(SUMSQ(C19, C29))</f>
-        <v>138.19207647329131</v>
-      </c>
-      <c r="D33">
-        <f t="shared" si="3"/>
-        <v>133.71970684981326</v>
-      </c>
-      <c r="E33">
-        <f t="shared" si="3"/>
-        <v>202.08649138425852</v>
-      </c>
-    </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
+        <v>25</v>
+      </c>
+      <c r="B34">
+        <f>SQRT(SUMSQ(B20, B30))</f>
+        <v>144.0783120389741</v>
+      </c>
+      <c r="C34">
+        <f t="shared" ref="C34:E34" si="3">SQRT(SUMSQ(C20, C30))</f>
+        <v>138.64519465167191</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="3"/>
+        <v>134.22190581272491</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="3"/>
+        <v>202.75897020847188</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>28</v>
       </c>
-      <c r="B34">
-        <f>SQRT(SUMSQ(B19, B30))</f>
-        <v>86.651947468017141</v>
-      </c>
-      <c r="C34">
-        <f t="shared" ref="C34:E34" si="4">SQRT(SUMSQ(C19, C30))</f>
-        <v>76.62930248932193</v>
-      </c>
-      <c r="D34">
+      <c r="B35">
+        <f>SQRT(SUMSQ(B20, B31))</f>
+        <v>86.796082860921786</v>
+      </c>
+      <c r="C35">
+        <f t="shared" ref="C35:E35" si="4">SQRT(SUMSQ(C20, C31))</f>
+        <v>77.443463249005077</v>
+      </c>
+      <c r="D35">
         <f t="shared" si="4"/>
-        <v>68.234595331107514</v>
-      </c>
-      <c r="E34">
+        <v>69.21358248205334</v>
+      </c>
+      <c r="E35">
         <f t="shared" si="4"/>
-        <v>91.863757815582531</v>
+        <v>93.333809522594763</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Put in last of James' edits barring some lost muons stuff.
</commit_message>
<xml_diff>
--- a/OtherMaterials/TotalSystematicErrorTable.xlsx
+++ b/OtherMaterials/TotalSystematicErrorTable.xlsx
@@ -1,23 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28502"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/NickPC/Documents/Graduation/Dissertation/OtherMaterials/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/NickPC/Documents/GraduationRequirements/Dissertation/OtherMaterials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E252738-BCA6-834F-804D-A84D11F7DC1F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="19100" windowWidth="24000" windowHeight="17440" xr2:uid="{13A7CC7D-E5DD-B54B-89F5-9477BBEDF731}"/>
+    <workbookView xWindow="1600" yWindow="460" windowWidth="24000" windowHeight="15540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -129,7 +134,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -484,11 +489,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17BA3B4E-0A14-7A4E-8738-91C0E27ED45A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -714,23 +719,23 @@
       </c>
       <c r="I13">
         <f>SQRT(SUMSQ(I5,B34))</f>
-        <v>1365.7211172124416</v>
+        <v>1365.7207803940012</v>
       </c>
       <c r="J13">
         <f t="shared" ref="J13:L13" si="0">SQRT(SUMSQ(J5,C34))</f>
-        <v>1417.9943335570845</v>
+        <v>1417.9940091551869</v>
       </c>
       <c r="K13">
         <f t="shared" si="0"/>
-        <v>913.21761371537286</v>
+        <v>913.21711000177822</v>
       </c>
       <c r="L13">
         <f t="shared" si="0"/>
-        <v>670.68300261748095</v>
+        <v>670.68231674914455</v>
       </c>
       <c r="N13" s="2">
         <f>SQRT(1/(1/(I13^2) + 1/(J13^2) +  1/(K13^2) +  1/(L13^2)))</f>
-        <v>473.74234828724633</v>
+        <v>473.74201008850446</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
@@ -772,16 +777,16 @@
         <v>17</v>
       </c>
       <c r="B16">
-        <v>2.4</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="C16">
-        <v>2.4</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="D16">
-        <v>2.4</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E16">
-        <v>2.4</v>
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -824,19 +829,19 @@
       </c>
       <c r="B20">
         <f>SQRT(SUMSQ(B6:B18))</f>
-        <v>41.31149960967285</v>
+        <v>41.300363194528934</v>
       </c>
       <c r="C20">
         <f t="shared" ref="C20:E20" si="1">SQRT(SUMSQ(C6:C18))</f>
-        <v>46.418099918027671</v>
+        <v>46.408188932558019</v>
       </c>
       <c r="D20">
         <f t="shared" si="1"/>
-        <v>27.76310501366877</v>
+        <v>27.74653131474275</v>
       </c>
       <c r="E20">
         <f t="shared" si="1"/>
-        <v>52.16617678151237</v>
+        <v>52.157358061926416</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -977,19 +982,19 @@
       </c>
       <c r="B34">
         <f>SQRT(SUMSQ(B20, B30))</f>
-        <v>144.0783120389741</v>
+        <v>144.0751192954564</v>
       </c>
       <c r="C34">
         <f t="shared" ref="C34:E34" si="3">SQRT(SUMSQ(C20, C30))</f>
-        <v>138.64519465167191</v>
+        <v>138.64187679052819</v>
       </c>
       <c r="D34">
         <f t="shared" si="3"/>
-        <v>134.22190581272491</v>
+        <v>134.21847860857312</v>
       </c>
       <c r="E34">
         <f t="shared" si="3"/>
-        <v>202.75897020847188</v>
+        <v>202.75670149220713</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
@@ -998,19 +1003,19 @@
       </c>
       <c r="B35">
         <f>SQRT(SUMSQ(B20, B31))</f>
-        <v>86.796082860921786</v>
+        <v>86.790782920768734</v>
       </c>
       <c r="C35">
         <f t="shared" ref="C35:E35" si="4">SQRT(SUMSQ(C20, C31))</f>
-        <v>77.443463249005077</v>
+        <v>77.437523204193454</v>
       </c>
       <c r="D35">
         <f t="shared" si="4"/>
-        <v>69.21358248205334</v>
+        <v>69.206936068576255</v>
       </c>
       <c r="E35">
         <f t="shared" si="4"/>
-        <v>93.333809522594763</v>
+        <v>93.328880846177512</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated differential decay error and beam motion error, adjusted associated text, table, and final numbers.
</commit_message>
<xml_diff>
--- a/OtherMaterials/TotalSystematicErrorTable.xlsx
+++ b/OtherMaterials/TotalSystematicErrorTable.xlsx
@@ -1,29 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28502"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11111"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/NickPC/Documents/GraduationRequirements/Dissertation/OtherMaterials/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/NickPC/Documents/Graduation/Dissertation/OtherMaterials/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FAABF19-A922-DC4D-B939-1AB57B3FF744}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1600" yWindow="460" windowWidth="24000" windowHeight="15540"/>
+    <workbookView xWindow="38400" yWindow="460" windowWidth="24000" windowHeight="37940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -134,7 +135,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -489,11 +490,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -719,23 +720,23 @@
       </c>
       <c r="I13">
         <f>SQRT(SUMSQ(I5,B34))</f>
-        <v>1365.7207803940012</v>
+        <v>1372.8544168993301</v>
       </c>
       <c r="J13">
         <f t="shared" ref="J13:L13" si="0">SQRT(SUMSQ(J5,C34))</f>
-        <v>1417.9940091551869</v>
+        <v>1424.8659621171389</v>
       </c>
       <c r="K13">
         <f t="shared" si="0"/>
-        <v>913.21711000177822</v>
+        <v>923.8514436856176</v>
       </c>
       <c r="L13">
         <f t="shared" si="0"/>
-        <v>670.68231674914455</v>
+        <v>686.46833138900149</v>
       </c>
       <c r="N13" s="2">
         <f>SQRT(1/(1/(I13^2) + 1/(J13^2) +  1/(K13^2) +  1/(L13^2)))</f>
-        <v>473.74201008850446</v>
+        <v>481.30113948456346</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
@@ -922,16 +923,16 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>115</v>
+        <v>181</v>
       </c>
       <c r="C28">
-        <v>115</v>
+        <v>181</v>
       </c>
       <c r="D28">
-        <v>115</v>
+        <v>181</v>
       </c>
       <c r="E28">
-        <v>180</v>
+        <v>232</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -940,19 +941,19 @@
       </c>
       <c r="B30">
         <f>SQRT(SUMSQ(B24:B28))</f>
-        <v>138.02869266931421</v>
+        <v>196.43808184769063</v>
       </c>
       <c r="C30">
         <f>SQRT(SUMSQ(C24:C28))</f>
-        <v>130.64398187440551</v>
+        <v>191.32132656868131</v>
       </c>
       <c r="D30">
         <f>SQRT(SUMSQ(D24:D28))</f>
-        <v>131.3191912859655</v>
+        <v>191.78302844621055</v>
       </c>
       <c r="E30">
         <f>SQRT(SUMSQ(E24:E28))</f>
-        <v>195.93338153566378</v>
+        <v>244.56878378075973</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -982,19 +983,19 @@
       </c>
       <c r="B34">
         <f>SQRT(SUMSQ(B20, B30))</f>
-        <v>144.0751192954564</v>
+        <v>200.7327576655091</v>
       </c>
       <c r="C34">
         <f t="shared" ref="C34:E34" si="3">SQRT(SUMSQ(C20, C30))</f>
-        <v>138.64187679052819</v>
+        <v>196.86942373055297</v>
       </c>
       <c r="D34">
         <f t="shared" si="3"/>
-        <v>134.21847860857312</v>
+        <v>193.77977190615124</v>
       </c>
       <c r="E34">
         <f t="shared" si="3"/>
-        <v>202.75670149220713</v>
+        <v>250.06855060163005</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Saving last iteration of systematics table excel sheet.
</commit_message>
<xml_diff>
--- a/OtherMaterials/TotalSystematicErrorTable.xlsx
+++ b/OtherMaterials/TotalSystematicErrorTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/NickPC/Documents/Graduation/Dissertation/OtherMaterials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FAABF19-A922-DC4D-B939-1AB57B3FF744}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD604BE5-300E-D84E-850F-67C507C804EF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38400" yWindow="460" windowWidth="24000" windowHeight="37940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -494,7 +494,7 @@
   <dimension ref="A1:N35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -720,23 +720,23 @@
       </c>
       <c r="I13">
         <f>SQRT(SUMSQ(I5,B34))</f>
-        <v>1372.8544168993301</v>
+        <v>1361.0632792049014</v>
       </c>
       <c r="J13">
         <f t="shared" ref="J13:L13" si="0">SQRT(SUMSQ(J5,C34))</f>
-        <v>1424.8659621171389</v>
+        <v>1413.5087583739976</v>
       </c>
       <c r="K13">
         <f t="shared" si="0"/>
-        <v>923.8514436856176</v>
+        <v>906.23699438943663</v>
       </c>
       <c r="L13">
         <f t="shared" si="0"/>
-        <v>686.46833138900149</v>
+        <v>647.51738972787439</v>
       </c>
       <c r="N13" s="2">
         <f>SQRT(1/(1/(I13^2) + 1/(J13^2) +  1/(K13^2) +  1/(L13^2)))</f>
-        <v>481.30113948456346</v>
+        <v>464.0886988219259</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
@@ -872,16 +872,16 @@
         <v>21</v>
       </c>
       <c r="B25">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C25">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="D25">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="E25">
-        <v>40</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -923,16 +923,16 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>181</v>
+        <v>45</v>
       </c>
       <c r="C28">
-        <v>181</v>
+        <v>45</v>
       </c>
       <c r="D28">
-        <v>181</v>
+        <v>45</v>
       </c>
       <c r="E28">
-        <v>232</v>
+        <v>58</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -941,19 +941,19 @@
       </c>
       <c r="B30">
         <f>SQRT(SUMSQ(B24:B28))</f>
-        <v>196.43808184769063</v>
+        <v>79.698933493491623</v>
       </c>
       <c r="C30">
         <f>SQRT(SUMSQ(C24:C28))</f>
-        <v>191.32132656868131</v>
+        <v>66.089711756066848</v>
       </c>
       <c r="D30">
         <f>SQRT(SUMSQ(D24:D28))</f>
-        <v>191.78302844621055</v>
+        <v>67.414612659274397</v>
       </c>
       <c r="E30">
         <f>SQRT(SUMSQ(E24:E28))</f>
-        <v>244.56878378075973</v>
+        <v>88.622175554428821</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -962,19 +962,19 @@
       </c>
       <c r="B31">
         <f>SQRT(SUMSQ(B24:B27))</f>
-        <v>76.334264914257218</v>
+        <v>65.779328059809188</v>
       </c>
       <c r="C31">
         <f t="shared" ref="C31:E31" si="2">SQRT(SUMSQ(C24:C27))</f>
-        <v>61.990725112713434</v>
+        <v>48.402995775055082</v>
       </c>
       <c r="D31">
         <f t="shared" si="2"/>
-        <v>63.401340679831058</v>
+        <v>50.196912255635809</v>
       </c>
       <c r="E31">
         <f t="shared" si="2"/>
-        <v>77.394379640901576</v>
+        <v>67.006641461873016</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
@@ -983,19 +983,19 @@
       </c>
       <c r="B34">
         <f>SQRT(SUMSQ(B20, B30))</f>
-        <v>200.7327576655091</v>
+        <v>89.764358182967044</v>
       </c>
       <c r="C34">
         <f t="shared" ref="C34:E34" si="3">SQRT(SUMSQ(C20, C30))</f>
-        <v>196.86942373055297</v>
+        <v>80.756238149136209</v>
       </c>
       <c r="D34">
         <f t="shared" si="3"/>
-        <v>193.77977190615124</v>
+        <v>72.901303143359513</v>
       </c>
       <c r="E34">
         <f t="shared" si="3"/>
-        <v>250.06855060163005</v>
+        <v>102.8313181866303</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
@@ -1004,19 +1004,19 @@
       </c>
       <c r="B35">
         <f>SQRT(SUMSQ(B20, B31))</f>
-        <v>86.790782920768734</v>
+        <v>77.670071456127815</v>
       </c>
       <c r="C35">
         <f t="shared" ref="C35:E35" si="4">SQRT(SUMSQ(C20, C31))</f>
-        <v>77.437523204193454</v>
+        <v>67.056468740905231</v>
       </c>
       <c r="D35">
         <f t="shared" si="4"/>
-        <v>69.206936068576255</v>
+        <v>57.355034652591748</v>
       </c>
       <c r="E35">
         <f t="shared" si="4"/>
-        <v>93.328880846177512</v>
+        <v>84.913367616647975</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Put in Rob's chapter 4 edits, took out bad chisq picture, and reformatted the chapter.
</commit_message>
<xml_diff>
--- a/OtherMaterials/TotalSystematicErrorTable.xlsx
+++ b/OtherMaterials/TotalSystematicErrorTable.xlsx
@@ -1,37 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11111"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28502"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/NickPC/Documents/Graduation/Dissertation/OtherMaterials/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/NickPC/Documents/GraduationRequirements/Dissertation/OtherMaterials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD604BE5-300E-D84E-850F-67C507C804EF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="460" windowWidth="24000" windowHeight="37940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1600" yWindow="460" windowWidth="24000" windowHeight="15540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="38">
   <si>
     <t>Total systematic error table</t>
   </si>
@@ -130,12 +129,27 @@
   </si>
   <si>
     <t>In-fill gain lifetime</t>
+  </si>
+  <si>
+    <t>Frequencies in rad/s</t>
+  </si>
+  <si>
+    <t>Average R values</t>
+  </si>
+  <si>
+    <t>Statistical error</t>
+  </si>
+  <si>
+    <t>Systematic error</t>
+  </si>
+  <si>
+    <t>Total error</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -490,18 +504,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="36.6640625" customWidth="1"/>
+    <col min="8" max="8" width="18.5" customWidth="1"/>
     <col min="9" max="9" width="16.1640625" customWidth="1"/>
-    <col min="12" max="12" width="11.83203125" customWidth="1"/>
+    <col min="10" max="10" width="13.1640625" customWidth="1"/>
+    <col min="11" max="12" width="13.5" customWidth="1"/>
     <col min="14" max="14" width="18" customWidth="1"/>
   </cols>
   <sheetData>
@@ -790,7 +806,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -807,7 +823,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -824,7 +840,21 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -844,13 +874,89 @@
         <f t="shared" si="1"/>
         <v>52.157358061926416</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H20" t="s">
+        <v>34</v>
+      </c>
+      <c r="I20">
+        <v>-20.5562</v>
+      </c>
+      <c r="J20">
+        <v>-17.4755</v>
+      </c>
+      <c r="K20">
+        <v>-17.7182</v>
+      </c>
+      <c r="L20">
+        <v>-17.340599999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H21" t="s">
+        <v>33</v>
+      </c>
+      <c r="I21">
+        <f>1000000 * 0.2291 * 2 * PI() * (1 + I20 * 0.000001)</f>
+        <v>1439448.1636822391</v>
+      </c>
+      <c r="J21">
+        <f t="shared" ref="J21:L21" si="2">1000000 * 0.2291 * 2 * PI() * (1 + J20 * 0.000001)</f>
+        <v>1439452.5982813553</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="2"/>
+        <v>1439452.2489201047</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="2"/>
+        <v>1439452.7924669043</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H22" t="s">
+        <v>35</v>
+      </c>
+      <c r="I22">
+        <f>1000000 * 0.2291 * 2 * PI() * (I5 * 0.001 * 0.000001)</f>
+        <v>1.9549547375374243</v>
+      </c>
+      <c r="J22">
+        <f t="shared" ref="J22:L22" si="3">1000000 * 0.2291 * 2 * PI() * (J5 * 0.001 * 0.000001)</f>
+        <v>2.0313910062681786</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="3"/>
+        <v>1.300280255075146</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="3"/>
+        <v>0.92025812805218721</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H23" t="s">
+        <v>36</v>
+      </c>
+      <c r="I23">
+        <f>1000000 * 0.2291 * 2 * PI() * (B34 * 0.001 * 0.000001)</f>
+        <v>0.12921379669523431</v>
+      </c>
+      <c r="J23">
+        <f t="shared" ref="J23:L23" si="4">1000000 * 0.2291 * 2 * PI() * (C34 * 0.001 * 0.000001)</f>
+        <v>0.11624680830230051</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="4"/>
+        <v>0.10493980410335221</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="4"/>
+        <v>0.14802339493127989</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>20</v>
       </c>
@@ -866,8 +972,27 @@
       <c r="E24">
         <v>58</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H24" t="s">
+        <v>37</v>
+      </c>
+      <c r="I24">
+        <f>1000000 * 0.2291 * 2 * PI() * (I13 * 0.001 * 0.000001)</f>
+        <v>1.9592203120314</v>
+      </c>
+      <c r="J24">
+        <f t="shared" ref="J24:L24" si="5">1000000 * 0.2291 * 2 * PI() * (J13 * 0.001 * 0.000001)</f>
+        <v>2.0347144125866206</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="5"/>
+        <v>1.3045079931619952</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="5"/>
+        <v>0.93208687776038213</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -884,7 +1009,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>22</v>
       </c>
@@ -901,7 +1026,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>23</v>
       </c>
@@ -918,7 +1043,7 @@
         <v>28.3</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -935,7 +1060,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>24</v>
       </c>
@@ -956,7 +1081,7 @@
         <v>88.622175554428821</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>27</v>
       </c>
@@ -965,15 +1090,15 @@
         <v>65.779328059809188</v>
       </c>
       <c r="C31">
-        <f t="shared" ref="C31:E31" si="2">SQRT(SUMSQ(C24:C27))</f>
+        <f t="shared" ref="C31:E31" si="6">SQRT(SUMSQ(C24:C27))</f>
         <v>48.402995775055082</v>
       </c>
       <c r="D31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>50.196912255635809</v>
       </c>
       <c r="E31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>67.006641461873016</v>
       </c>
     </row>
@@ -986,15 +1111,15 @@
         <v>89.764358182967044</v>
       </c>
       <c r="C34">
-        <f t="shared" ref="C34:E34" si="3">SQRT(SUMSQ(C20, C30))</f>
+        <f t="shared" ref="C34:E34" si="7">SQRT(SUMSQ(C20, C30))</f>
         <v>80.756238149136209</v>
       </c>
       <c r="D34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>72.901303143359513</v>
       </c>
       <c r="E34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>102.8313181866303</v>
       </c>
     </row>
@@ -1007,15 +1132,15 @@
         <v>77.670071456127815</v>
       </c>
       <c r="C35">
-        <f t="shared" ref="C35:E35" si="4">SQRT(SUMSQ(C20, C31))</f>
+        <f t="shared" ref="C35:E35" si="8">SQRT(SUMSQ(C20, C31))</f>
         <v>67.056468740905231</v>
       </c>
       <c r="D35">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>57.355034652591748</v>
       </c>
       <c r="E35">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>84.913367616647975</v>
       </c>
     </row>

</xml_diff>